<commit_message>
local changes from eons ago
</commit_message>
<xml_diff>
--- a/productgenerator/productgen/productgen.xlsx
+++ b/productgenerator/productgen/productgen.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Brands</t>
   </si>
@@ -89,10 +89,16 @@
     <t>Louise Veeton</t>
   </si>
   <si>
-    <t>Prat-a</t>
-  </si>
-  <si>
     <t>hand made</t>
+  </si>
+  <si>
+    <t>Timmy Hellfire</t>
+  </si>
+  <si>
+    <t>purple</t>
+  </si>
+  <si>
+    <t>Viveeon Eastwood</t>
   </si>
 </sst>
 </file>
@@ -453,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,7 +502,7 @@
         <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -518,7 +524,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
@@ -539,6 +545,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
@@ -546,6 +555,11 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>